<commit_message>
EPBDS-8319 SmartRules: Adding missing functionalities
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8319_Simple_and_Smart_Rules_Several_RET.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8319_Simple_and_Smart_Rules_Several_RET.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkamalov\.openl\user-workspace\DEFAULT\EPBDS-8319_Simple_and_Smart_Rules_Several_RET\"/>
     </mc:Choice>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="104">
   <si>
     <t>SmartRules Collect Double[] testSmartRules (Integer a, String b)</t>
   </si>
@@ -340,10 +340,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -367,15 +368,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -750,9 +755,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -1356,7 +1361,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10BC802E-D377-44AB-B656-A50E0FA00DD2}">
-  <dimension ref="C4:H53"/>
+  <dimension ref="C4:G53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:H9"/>
@@ -1364,10 +1369,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
@@ -1554,6 +1559,7 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
@@ -1568,10 +1574,7 @@
       <c r="F40" t="s">
         <v>42</v>
       </c>
-      <c r="G40" t="s">
-        <v>43</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="G40" t="s" s="0">
         <v>47</v>
       </c>
     </row>
@@ -1582,8 +1585,7 @@
       <c r="D41" t="s">
         <v>2</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41">
+      <c r="G41" t="n" s="0">
         <v>1.4</v>
       </c>
     </row>
@@ -1597,6 +1599,7 @@
       <c r="E42" t="s">
         <v>5</v>
       </c>
+      <c r="G42" s="6"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43">
@@ -1605,9 +1608,10 @@
       <c r="D43" t="s">
         <v>3</v>
       </c>
-      <c r="G43" t="s">
+      <c r="F43" t="s">
         <v>6</v>
       </c>
+      <c r="G43" s="5"/>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44">
@@ -1619,9 +1623,7 @@
       <c r="F44" t="s">
         <v>4</v>
       </c>
-      <c r="G44" t="s">
-        <v>4</v>
-      </c>
+      <c r="G44" s="4"/>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
@@ -1709,9 +1711,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="45.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="45.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="45.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -1852,8 +1854,8 @@
       <c r="D30" t="s">
         <v>72</v>
       </c>
-      <c r="E30" t="s">
-        <v>27</v>
+      <c r="E30" t="n">
+        <v>5.0</v>
       </c>
       <c r="F30" t="s">
         <v>75</v>
@@ -1872,8 +1874,8 @@
       <c r="D31" t="s">
         <v>72</v>
       </c>
-      <c r="E31" t="s">
-        <v>77</v>
+      <c r="E31" t="n">
+        <v>6.0</v>
       </c>
       <c r="F31" t="s">
         <v>78</v>
@@ -1892,8 +1894,8 @@
       <c r="D32" t="s">
         <v>72</v>
       </c>
-      <c r="E32" t="s">
-        <v>80</v>
+      <c r="E32" t="n">
+        <v>7.0</v>
       </c>
       <c r="F32" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
EPBDS-8671 No validation of type of Map return result for Smart and Simple rules
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8319_Simple_and_Smart_Rules_Several_RET.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8319_Simple_and_Smart_Rules_Several_RET.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkamalov\.openl\user-workspace\DEFAULT\EPBDS-8319_Simple_and_Smart_Rules_Several_RET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C456605-CFB4-4F2D-863D-FC0DCA857EDD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94011B6-62D6-4704-B0BC-947D35306139}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="1290" windowWidth="31485" windowHeight="15300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1395" yWindow="180" windowWidth="26505" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="104">
   <si>
     <t>SmartRules Collect Double[] testSmartRules (Integer a, String b)</t>
   </si>
@@ -84,9 +84,6 @@
     <t>SimpleRules  Collect Double[] testSimpleRules (Integer a, String b)</t>
   </si>
   <si>
-    <t>SmartRules  Collect as Double and Double Map testSmartRulesMap1 (Integer a, String b)</t>
-  </si>
-  <si>
     <t>SimpleRules  Collect as String and Double Map testSimpleRulesMap2 (Integer a, String b)</t>
   </si>
   <si>
@@ -334,17 +331,19 @@
   </si>
   <si>
     <t>Test test2_3 test2_3Test</t>
+  </si>
+  <si>
+    <t>SmartRules  Collect as String and Double Map testSmartRulesMap1 (Integer a, String b)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -368,19 +367,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -749,24 +747,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B6:G77"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:F69"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -830,12 +828,12 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -845,10 +843,10 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
         <v>33</v>
-      </c>
-      <c r="E16" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -902,13 +900,13 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="B27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -935,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F29" t="s">
         <v>5</v>
@@ -949,7 +947,7 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
@@ -963,7 +961,7 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -980,7 +978,7 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
@@ -990,13 +988,13 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="B38" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -1023,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F40" t="s">
         <v>5</v>
@@ -1037,7 +1035,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E41" t="s">
         <v>17</v>
@@ -1051,7 +1049,7 @@
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E42" t="s">
         <v>6</v>
@@ -1068,7 +1066,7 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E43" t="s">
         <v>4</v>
@@ -1078,14 +1076,14 @@
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
+      <c r="B45" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -1095,16 +1093,16 @@
         <v>12</v>
       </c>
       <c r="D46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" t="s">
         <v>28</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>29</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>30</v>
-      </c>
-      <c r="G46" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
@@ -1129,7 +1127,7 @@
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -1145,14 +1143,14 @@
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
+      <c r="B54" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
@@ -1162,16 +1160,16 @@
         <v>12</v>
       </c>
       <c r="D55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" t="s">
         <v>28</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>29</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>30</v>
-      </c>
-      <c r="G55" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -1196,7 +1194,7 @@
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
@@ -1369,60 +1367,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
@@ -1432,10 +1430,10 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
         <v>42</v>
-      </c>
-      <c r="F20" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
@@ -1487,7 +1485,7 @@
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
@@ -1541,7 +1539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>2</v>
       </c>
@@ -1552,16 +1550,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="7"/>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>1</v>
       </c>
@@ -1569,27 +1567,27 @@
         <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F40" t="s">
-        <v>42</v>
-      </c>
-      <c r="G40" t="s" s="0">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="G40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
         <v>2</v>
       </c>
-      <c r="G41" t="n" s="0">
+      <c r="G41">
         <v>1.4</v>
       </c>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>1</v>
       </c>
@@ -1599,9 +1597,9 @@
       <c r="E42" t="s">
         <v>5</v>
       </c>
-      <c r="G42" s="6"/>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>2</v>
       </c>
@@ -1611,9 +1609,9 @@
       <c r="F43" t="s">
         <v>6</v>
       </c>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>1</v>
       </c>
@@ -1623,11 +1621,11 @@
       <c r="F44" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="4"/>
+      <c r="G44" s="2"/>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
@@ -1705,132 +1703,133 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FD3D36-1C98-4741-BE52-9ACC241FAB6A}">
   <dimension ref="B4:J148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="45.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="45.5703125" collapsed="true"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="45.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
         <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
         <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
         <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
         <v>59</v>
-      </c>
-      <c r="C14" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
         <v>67</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>68</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>69</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>70</v>
-      </c>
-      <c r="F28" t="s">
-        <v>71</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
@@ -1841,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
@@ -1849,19 +1848,19 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
         <v>74</v>
       </c>
-      <c r="D30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>75</v>
-      </c>
       <c r="G30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1869,19 +1868,19 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" t="n">
-        <v>6.0</v>
+        <v>71</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -1889,49 +1888,49 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" t="n">
-        <v>7.0</v>
+        <v>71</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
       </c>
       <c r="F32" t="s">
+        <v>80</v>
+      </c>
+      <c r="G32" t="s">
         <v>81</v>
-      </c>
-      <c r="G32" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E43" t="s">
         <v>9</v>
@@ -1939,55 +1938,55 @@
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" t="s">
         <v>67</v>
       </c>
-      <c r="C50" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>68</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>69</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>70</v>
-      </c>
-      <c r="G50" t="s">
-        <v>71</v>
       </c>
       <c r="H50" t="s">
         <v>9</v>
@@ -1997,10 +1996,10 @@
       <c r="B51">
         <v>0</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I51" s="2"/>
+      <c r="H51" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I51" s="1"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52">
@@ -2010,21 +2009,21 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" t="s">
         <v>74</v>
       </c>
-      <c r="E52" t="s">
-        <v>93</v>
-      </c>
-      <c r="F52" t="s">
-        <v>27</v>
-      </c>
-      <c r="G52" t="s">
-        <v>75</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I52" s="2"/>
+      <c r="H52" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I52" s="1"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53">
@@ -2034,21 +2033,21 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" t="s">
+        <v>92</v>
+      </c>
+      <c r="F53" t="s">
         <v>76</v>
       </c>
-      <c r="E53" t="s">
-        <v>93</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>77</v>
       </c>
-      <c r="G53" t="s">
-        <v>78</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I53" s="2"/>
+      <c r="H53" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I53" s="1"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54">
@@ -2058,42 +2057,42 @@
         <v>3</v>
       </c>
       <c r="D54" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" t="s">
+        <v>92</v>
+      </c>
+      <c r="F54" t="s">
         <v>79</v>
       </c>
-      <c r="E54" t="s">
-        <v>93</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>80</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H54" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I54" s="2"/>
+      <c r="I54" s="1"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -2101,43 +2100,43 @@
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C68" t="s">
         <v>9</v>
       </c>
       <c r="D68" t="s">
+        <v>67</v>
+      </c>
+      <c r="E68" t="s">
         <v>68</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>69</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>70</v>
-      </c>
-      <c r="G68" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
@@ -2145,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="C69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
@@ -2153,16 +2152,16 @@
         <v>1</v>
       </c>
       <c r="D70" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" t="s">
+        <v>26</v>
+      </c>
+      <c r="G70" t="s">
         <v>74</v>
-      </c>
-      <c r="E70" t="s">
-        <v>72</v>
-      </c>
-      <c r="F70" t="s">
-        <v>27</v>
-      </c>
-      <c r="G70" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
@@ -2170,19 +2169,19 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D71" t="s">
+        <v>75</v>
+      </c>
+      <c r="E71" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" t="s">
         <v>76</v>
       </c>
-      <c r="E71" t="s">
-        <v>72</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>77</v>
-      </c>
-      <c r="G71" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
@@ -2190,49 +2189,49 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D72" t="s">
+        <v>78</v>
+      </c>
+      <c r="E72" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" t="s">
         <v>79</v>
       </c>
-      <c r="E72" t="s">
-        <v>72</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>80</v>
-      </c>
-      <c r="G72" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E78" t="s">
         <v>9</v>
@@ -2240,163 +2239,163 @@
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C86" t="s">
         <v>9</v>
       </c>
       <c r="D86" t="s">
+        <v>66</v>
+      </c>
+      <c r="E86" t="s">
         <v>67</v>
       </c>
-      <c r="E86" t="s">
+      <c r="F86" t="s">
         <v>68</v>
       </c>
-      <c r="F86" t="s">
+      <c r="G86" t="s">
         <v>69</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>70</v>
-      </c>
-      <c r="H86" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>0</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
+      <c r="C87" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>1</v>
       </c>
-      <c r="C88" s="2"/>
+      <c r="C88" s="1"/>
       <c r="D88">
         <v>1</v>
       </c>
       <c r="E88" t="s">
+        <v>73</v>
+      </c>
+      <c r="F88" t="s">
+        <v>92</v>
+      </c>
+      <c r="G88" t="s">
+        <v>26</v>
+      </c>
+      <c r="H88" t="s">
         <v>74</v>
       </c>
-      <c r="F88" t="s">
-        <v>93</v>
-      </c>
-      <c r="G88" t="s">
-        <v>27</v>
-      </c>
-      <c r="H88" t="s">
-        <v>75</v>
-      </c>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>2</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>82</v>
+      <c r="C89" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="D89">
         <v>2</v>
       </c>
       <c r="E89" t="s">
+        <v>75</v>
+      </c>
+      <c r="F89" t="s">
+        <v>92</v>
+      </c>
+      <c r="G89" t="s">
         <v>76</v>
       </c>
-      <c r="F89" t="s">
-        <v>93</v>
-      </c>
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>77</v>
       </c>
-      <c r="H89" t="s">
-        <v>78</v>
-      </c>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>3</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>82</v>
+      <c r="C90" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="D90">
         <v>3</v>
       </c>
       <c r="E90" t="s">
+        <v>78</v>
+      </c>
+      <c r="F90" t="s">
+        <v>92</v>
+      </c>
+      <c r="G90" t="s">
         <v>79</v>
       </c>
-      <c r="F90" t="s">
-        <v>93</v>
-      </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>80</v>
       </c>
-      <c r="H90" t="s">
-        <v>81</v>
-      </c>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C95" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C96" t="s">
         <v>9</v>
@@ -2404,43 +2403,43 @@
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C97" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C98" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
+        <v>66</v>
+      </c>
+      <c r="C103" t="s">
+        <v>99</v>
+      </c>
+      <c r="D103" t="s">
         <v>67</v>
       </c>
-      <c r="C103" t="s">
-        <v>100</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>68</v>
       </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
         <v>69</v>
       </c>
-      <c r="F103" t="s">
+      <c r="G103" t="s">
         <v>70</v>
-      </c>
-      <c r="G103" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
@@ -2448,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="C104" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
@@ -2456,16 +2455,16 @@
         <v>1</v>
       </c>
       <c r="D105" t="s">
+        <v>73</v>
+      </c>
+      <c r="E105" t="s">
+        <v>71</v>
+      </c>
+      <c r="F105" t="s">
+        <v>26</v>
+      </c>
+      <c r="G105" t="s">
         <v>74</v>
-      </c>
-      <c r="E105" t="s">
-        <v>72</v>
-      </c>
-      <c r="F105" t="s">
-        <v>27</v>
-      </c>
-      <c r="G105" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
@@ -2473,19 +2472,19 @@
         <v>2</v>
       </c>
       <c r="C106" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D106" t="s">
+        <v>75</v>
+      </c>
+      <c r="E106" t="s">
+        <v>71</v>
+      </c>
+      <c r="F106" t="s">
         <v>76</v>
       </c>
-      <c r="E106" t="s">
-        <v>72</v>
-      </c>
-      <c r="F106" t="s">
+      <c r="G106" t="s">
         <v>77</v>
-      </c>
-      <c r="G106" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
@@ -2493,49 +2492,49 @@
         <v>3</v>
       </c>
       <c r="C107" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D107" t="s">
+        <v>78</v>
+      </c>
+      <c r="E107" t="s">
+        <v>71</v>
+      </c>
+      <c r="F107" t="s">
         <v>79</v>
       </c>
-      <c r="E107" t="s">
-        <v>72</v>
-      </c>
-      <c r="F107" t="s">
+      <c r="G107" t="s">
         <v>80</v>
-      </c>
-      <c r="G107" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C113" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D113" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E113" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C114" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D114" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E114" t="s">
         <v>9</v>
@@ -2543,85 +2542,85 @@
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C115" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D115" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E115" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C116" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D116" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E116" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
+        <v>34</v>
+      </c>
+      <c r="C124" t="s">
         <v>35</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
         <v>36</v>
       </c>
-      <c r="D124" t="s">
+      <c r="E124" t="s">
         <v>37</v>
-      </c>
-      <c r="E124" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
+        <v>99</v>
+      </c>
+      <c r="C125" t="s">
         <v>100</v>
       </c>
-      <c r="C125" t="s">
-        <v>101</v>
-      </c>
       <c r="D125" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
+        <v>66</v>
+      </c>
+      <c r="C131" t="s">
         <v>67</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
         <v>68</v>
       </c>
-      <c r="D131" t="s">
+      <c r="E131" t="s">
         <v>69</v>
       </c>
-      <c r="E131" t="s">
+      <c r="F131" t="s">
         <v>70</v>
       </c>
-      <c r="F131" t="s">
-        <v>71</v>
-      </c>
       <c r="G131" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.25">
@@ -2629,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="G132" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.25">
@@ -2637,19 +2636,19 @@
         <v>1</v>
       </c>
       <c r="C133" t="s">
+        <v>73</v>
+      </c>
+      <c r="D133" t="s">
+        <v>71</v>
+      </c>
+      <c r="E133" t="s">
+        <v>26</v>
+      </c>
+      <c r="F133" t="s">
         <v>74</v>
       </c>
-      <c r="D133" t="s">
-        <v>72</v>
-      </c>
-      <c r="E133" t="s">
-        <v>27</v>
-      </c>
-      <c r="F133" t="s">
-        <v>75</v>
-      </c>
       <c r="G133" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
@@ -2657,19 +2656,19 @@
         <v>2</v>
       </c>
       <c r="C134" t="s">
+        <v>75</v>
+      </c>
+      <c r="D134" t="s">
+        <v>71</v>
+      </c>
+      <c r="E134" t="s">
         <v>76</v>
       </c>
-      <c r="D134" t="s">
-        <v>72</v>
-      </c>
-      <c r="E134" t="s">
+      <c r="F134" t="s">
         <v>77</v>
       </c>
-      <c r="F134" t="s">
-        <v>78</v>
-      </c>
       <c r="G134" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
@@ -2677,49 +2676,49 @@
         <v>3</v>
       </c>
       <c r="C135" t="s">
+        <v>78</v>
+      </c>
+      <c r="D135" t="s">
+        <v>71</v>
+      </c>
+      <c r="E135" t="s">
         <v>79</v>
       </c>
-      <c r="D135" t="s">
-        <v>72</v>
-      </c>
-      <c r="E135" t="s">
+      <c r="F135" t="s">
         <v>80</v>
       </c>
-      <c r="F135" t="s">
+      <c r="G135" t="s">
         <v>81</v>
-      </c>
-      <c r="G135" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C145" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D145" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E145" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C146" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D146" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E146" t="s">
         <v>9</v>
@@ -2727,30 +2726,30 @@
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C147" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D147" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E147" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C148" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D148" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E148" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>